<commit_message>
update BOM, add device purchase link
</commit_message>
<xml_diff>
--- a/Hardware/BOM/BOM_Board1_PCB1_2022-10-06.xlsx
+++ b/Hardware/BOM/BOM_Board1_PCB1_2022-10-06.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EE2ACE-D96E-40D1-BD26-A61DB13FB585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D5533-FB55-46EE-B6B3-88C47B0D1D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="116">
   <si>
     <t>Device</t>
   </si>
@@ -317,9 +317,6 @@
     <t>VL162</t>
   </si>
   <si>
-    <t>VL162 OK</t>
-  </si>
-  <si>
     <t>R33,R35,R26,R27,R28</t>
   </si>
   <si>
@@ -333,16 +330,57 @@
   </si>
   <si>
     <t>1.0H or 0.8H</t>
+  </si>
+  <si>
+    <t>Choose one of the U4, U8</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>For Test only, not mount</t>
+  </si>
+  <si>
+    <t>HDMI ESD</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a230r.1.14.16.3f467d3ael2qUa&amp;id=683231973073</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z10.3-c.w4002-318537838.9.634616c1ucYXw3&amp;id=686780305043</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z10.3-c.w4002-318537838.9.14c916c1FQ2ka6&amp;id=681747465422</t>
+  </si>
+  <si>
+    <t>Via-labs VL162</t>
+  </si>
+  <si>
+    <t>Can using VL160 instead, Change R13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,17 +403,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -715,14 +756,14 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="95.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,13 +832,13 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -822,6 +863,9 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -845,6 +889,9 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -868,6 +915,9 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -937,6 +987,9 @@
       <c r="G9" s="1">
         <v>4</v>
       </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -983,6 +1036,9 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1006,6 +1062,9 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1053,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,7 +1138,7 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,7 +1448,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
         <v>62</v>
@@ -1412,7 +1471,7 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
         <v>52</v>
@@ -1435,7 +1494,7 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
         <v>67</v>
@@ -1473,7 +1532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1519,7 +1578,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1542,7 +1601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1565,12 +1624,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{1782A412-C075-4BB7-9352-33E74D5AEA1B}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{3D4611CD-326C-430A-AC0F-DDC1FC5D4994}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{DA185D4F-3E50-41E9-8BE0-95851924D73A}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>